<commit_message>
changed name of databases
</commit_message>
<xml_diff>
--- a/coordinates_municipalities_extremadura.xlsx
+++ b/coordinates_municipalities_extremadura.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javiercanalesluna/Desktop/Documentos/Extremadura/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javiercanalesluna/Desktop/Documentos/repositories/covid19_extremadura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43C0D5A-5D9F-B847-B1A1-8522BEA32A18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1195AE-4C2F-C545-A7A1-6F5371E20ECC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,9 +1198,6 @@
     <t>ccaa</t>
   </si>
   <si>
-    <t>area_salud</t>
-  </si>
-  <si>
     <t>longitud</t>
   </si>
   <si>
@@ -1208,6 +1205,9 @@
   </si>
   <si>
     <t>municipio</t>
+  </si>
+  <si>
+    <t>area_salud_id</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2062,7 @@
   <dimension ref="A1:F390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2080,16 +2080,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D1" t="s">
         <v>394</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>391</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>392</v>
-      </c>
-      <c r="F1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>